<commit_message>
User Story 1 erweitert
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>User Stories</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>in Bearbeitung</t>
+  </si>
+  <si>
+    <t>Controller und Views für die Startseite erstellen</t>
   </si>
 </sst>
 </file>
@@ -562,10 +565,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +594,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -599,11 +602,16 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Layout.cshtml und Site.css erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>User Stories</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Controller und Views für die Startseite erstellen</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,22 +600,31 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UserStory 2 Tasks hinzugefügt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>User Stories</t>
   </si>
@@ -85,6 +85,24 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>Datenbank und Tabelle erstellen</t>
+  </si>
+  <si>
+    <t>Interface UserRepository erstellen</t>
+  </si>
+  <si>
+    <t>Klasse User erstellen</t>
+  </si>
+  <si>
+    <t>Klasse UserRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>Registration View erstellen</t>
+  </si>
+  <si>
+    <t>Registration Methode im UserController erstellen</t>
   </si>
 </sst>
 </file>
@@ -491,7 +509,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,10 +586,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +642,48 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Datenbank UserRepository.cs und User.cs hinzugefügt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>User Stories</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Grundlegendes Layout für Handy</t>
   </si>
   <si>
-    <t>Layout für PC und Handy verschönern</t>
-  </si>
-  <si>
-    <t>in Bearbeitung</t>
-  </si>
-  <si>
     <t>Controller und Views für die Startseite erstellen</t>
   </si>
   <si>
@@ -103,6 +97,18 @@
   </si>
   <si>
     <t>Registration Methode im UserController erstellen</t>
+  </si>
+  <si>
+    <t>b … in Bearbeitung</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Als Admin möchte ich einen eigenen Bereich, wo alle registrierten Benutzer angezeigt und verwaltet werden können</t>
+  </si>
+  <si>
+    <t>Als Benutzer möchte ich alle Seiten auf deutsch und englisch aufrufen können</t>
   </si>
 </sst>
 </file>
@@ -450,7 +456,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +502,7 @@
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -509,7 +515,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,12 +577,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -586,10 +592,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,12 +606,15 @@
     <col min="4" max="4" width="45.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -613,47 +622,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
@@ -661,29 +670,30 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UserController und Registration View erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>User Stories</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>b … in Bearbeitung</t>
-  </si>
-  <si>
-    <t>b</t>
   </si>
   <si>
     <t>Als Admin möchte ich einen eigenen Bereich, wo alle registrierten Benutzer angezeigt und verwaltet werden können</t>
@@ -502,7 +499,7 @@
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +579,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -595,7 +592,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,17 +680,23 @@
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Message.cs und Message.cshtml erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>User Stories</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Als Benutzer möchte ich alle Seiten auf deutsch und englisch aufrufen können</t>
+  </si>
+  <si>
+    <t>für Erfolgsseiten Klasse und View Message erstellen</t>
+  </si>
+  <si>
+    <t>abgeschlossen</t>
   </si>
 </sst>
 </file>
@@ -141,13 +147,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,7 +521,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,10 +598,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,18 +609,24 @@
     <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="50.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -619,31 +634,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="3">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="3">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="3">
+        <v>43517</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -651,52 +675,81 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="3">
+        <v>43522</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="3">
+        <v>43522</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="3">
+        <v>43522</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <v>43522</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="3">
+        <v>43522</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
+      </c>
+      <c r="D14" s="3">
+        <v>43522</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="3">
+        <v>43525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UserStory 3 Tasks erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>User Stories</t>
   </si>
@@ -108,10 +108,31 @@
     <t>Als Benutzer möchte ich alle Seiten auf deutsch und englisch aufrufen können</t>
   </si>
   <si>
+    <t>b</t>
+  </si>
+  <si>
     <t>für Erfolgsseiten Klasse und View Message erstellen</t>
   </si>
   <si>
-    <t>abgeschlossen</t>
+    <t>Zustand</t>
+  </si>
+  <si>
+    <t>abgeschlossen am</t>
+  </si>
+  <si>
+    <t>IUserRepository und UserRepositoryDB erweitern</t>
+  </si>
+  <si>
+    <t>Login Methode im UserConroller erstellen (inkl. Sessions)</t>
+  </si>
+  <si>
+    <t>Logout Methode im UserController erstellen</t>
+  </si>
+  <si>
+    <t>Klasse Login erstellen</t>
+  </si>
+  <si>
+    <t>Login View erstellen</t>
   </si>
 </sst>
 </file>
@@ -521,7 +542,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,18 +619,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="55.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -617,8 +638,11 @@
       <c r="A1" t="s">
         <v>16</v>
       </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -743,13 +767,49 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="3">
         <v>43525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Login.cs erstellt; IUserRepository und UserRepositoryDB erweitert
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>User Stories</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Als Benutzer möchte ich alle Seiten auf deutsch und englisch aufrufen können</t>
-  </si>
-  <si>
-    <t>b</t>
   </si>
   <si>
     <t>für Erfolgsseiten Klasse und View Message erstellen</t>
@@ -622,7 +619,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,10 +636,10 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -767,7 +764,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -776,7 +773,7 @@
         <v>43525</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -784,32 +781,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="3">
+        <v>43525</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UserController erweitert und Login.cshtml erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>User Stories</t>
   </si>
@@ -120,9 +120,6 @@
     <t>IUserRepository und UserRepositoryDB erweitern</t>
   </si>
   <si>
-    <t>Login Methode im UserConroller erstellen (inkl. Sessions)</t>
-  </si>
-  <si>
     <t>Logout Methode im UserController erstellen</t>
   </si>
   <si>
@@ -130,6 +127,12 @@
   </si>
   <si>
     <t>Login View erstellen</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Login Methode im UserController erstellen (inkl. Sessions)</t>
   </si>
 </sst>
 </file>
@@ -618,14 +621,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="55.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
@@ -783,7 +786,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
@@ -796,20 +799,41 @@
       <c r="B19" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="3">
+        <v>43530</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="3">
+        <v>43530</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="3">
+        <v>43530</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logout Methode im UserController erstellt und Layout für Anmeldung angepasst
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="UserStories" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>User Stories</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>Login View erstellen</t>
-  </si>
-  <si>
-    <t>b</t>
   </si>
   <si>
     <t>Login Methode im UserController erstellen (inkl. Sessions)</t>
@@ -482,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +805,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
@@ -833,7 +830,10 @@
         <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+      <c r="D22" s="3">
+        <v>43530</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UserStories erweitert und UserStory 4 Tasks erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="UserStories" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
   <si>
     <t>User Stories</t>
   </si>
@@ -63,9 +63,6 @@
     <t>7.</t>
   </si>
   <si>
-    <t>Als Admin möchte ich einen eigenen Bereich, wo alle registrierten Benutzer angezeigt werden</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>abgeschlossen am</t>
   </si>
   <si>
-    <t>IUserRepository und UserRepositoryDB erweitern</t>
-  </si>
-  <si>
     <t>Logout Methode im UserController erstellen</t>
   </si>
   <si>
@@ -129,7 +123,40 @@
     <t>Login View erstellen</t>
   </si>
   <si>
+    <t>b</t>
+  </si>
+  <si>
     <t>Login Methode im UserController erstellen (inkl. Sessions)</t>
+  </si>
+  <si>
+    <t>IUserRepository und UserRepositoryDB erweitern (Authenticate)</t>
+  </si>
+  <si>
+    <t>Als registrierter Benutzer möchte ich mein Profil ändern wenn ich mich angemeldet habe</t>
+  </si>
+  <si>
+    <t>8.</t>
+  </si>
+  <si>
+    <t>Navigations-Menü für Anmeldung erweitern</t>
+  </si>
+  <si>
+    <t>ChangeUserData Methode im UserController erstellen</t>
+  </si>
+  <si>
+    <t>IUserRepository und UserRepositoryDB erweitern (ChangeUserData)</t>
+  </si>
+  <si>
+    <t>ChangeUserData View erstellen</t>
+  </si>
+  <si>
+    <t>IUserRepository und UserRepositoryDB erweitern (ChangePassword)</t>
+  </si>
+  <si>
+    <t>ChangePassword Methode im UserController erstellen</t>
+  </si>
+  <si>
+    <t>ChangePassword View erstellen</t>
   </si>
 </sst>
 </file>
@@ -477,16 +504,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -516,7 +543,7 @@
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -526,7 +553,12 @@
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -536,16 +568,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -582,7 +614,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -590,7 +622,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -598,15 +630,23 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -616,16 +656,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="61" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
@@ -633,18 +673,18 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -657,10 +697,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3">
         <v>43515</v>
@@ -668,10 +708,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3">
         <v>43515</v>
@@ -679,10 +719,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3">
         <v>43517</v>
@@ -698,10 +738,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3">
         <v>43522</v>
@@ -709,10 +749,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3">
         <v>43522</v>
@@ -720,10 +760,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3">
         <v>43522</v>
@@ -731,10 +771,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3">
         <v>43522</v>
@@ -742,10 +782,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="3">
         <v>43522</v>
@@ -753,10 +793,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="3">
         <v>43522</v>
@@ -764,10 +804,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="3">
         <v>43525</v>
@@ -783,10 +823,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="3">
         <v>43525</v>
@@ -794,10 +834,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="3">
         <v>43530</v>
@@ -805,10 +845,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="3">
         <v>43530</v>
@@ -816,10 +856,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="3">
         <v>43530</v>
@@ -827,13 +867,65 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="3">
         <v>43530</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3">
+        <v>43530</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IUserRepository und UserRepositoryDB erweitert (GetUser)
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -144,9 +144,6 @@
     <t>ChangeUserData Methode im UserController erstellen</t>
   </si>
   <si>
-    <t>IUserRepository und UserRepositoryDB erweitern (ChangeUserData)</t>
-  </si>
-  <si>
     <t>ChangeUserData View erstellen</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>ChangePassword View erstellen</t>
+  </si>
+  <si>
+    <t>IUserRepository und UserRepositoryDB erweitern (ChangeUserData und GetUser)</t>
   </si>
 </sst>
 </file>
@@ -659,7 +659,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,9 +895,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
         <v>35</v>
@@ -910,22 +910,22 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UserController erweitert und ChangeUserData.cshtml erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>User Stories</t>
   </si>
@@ -123,40 +123,43 @@
     <t>Login View erstellen</t>
   </si>
   <si>
+    <t>Login Methode im UserController erstellen (inkl. Sessions)</t>
+  </si>
+  <si>
+    <t>IUserRepository und UserRepositoryDB erweitern (Authenticate)</t>
+  </si>
+  <si>
+    <t>Als registrierter Benutzer möchte ich mein Profil ändern wenn ich mich angemeldet habe</t>
+  </si>
+  <si>
+    <t>8.</t>
+  </si>
+  <si>
+    <t>Navigations-Menü für Anmeldung erweitern</t>
+  </si>
+  <si>
+    <t>ChangeUserData Methode im UserController erstellen</t>
+  </si>
+  <si>
+    <t>ChangeUserData View erstellen</t>
+  </si>
+  <si>
+    <t>IUserRepository und UserRepositoryDB erweitern (ChangePassword)</t>
+  </si>
+  <si>
+    <t>ChangePassword Methode im UserController erstellen</t>
+  </si>
+  <si>
+    <t>ChangePassword View erstellen</t>
+  </si>
+  <si>
+    <t>IUserRepository und UserRepositoryDB erweitern (ChangeUserData und GetUser)</t>
+  </si>
+  <si>
+    <t>Navigations-Menü für Zugriff auf das Profil erweitern</t>
+  </si>
+  <si>
     <t>b</t>
-  </si>
-  <si>
-    <t>Login Methode im UserController erstellen (inkl. Sessions)</t>
-  </si>
-  <si>
-    <t>IUserRepository und UserRepositoryDB erweitern (Authenticate)</t>
-  </si>
-  <si>
-    <t>Als registrierter Benutzer möchte ich mein Profil ändern wenn ich mich angemeldet habe</t>
-  </si>
-  <si>
-    <t>8.</t>
-  </si>
-  <si>
-    <t>Navigations-Menü für Anmeldung erweitern</t>
-  </si>
-  <si>
-    <t>ChangeUserData Methode im UserController erstellen</t>
-  </si>
-  <si>
-    <t>ChangeUserData View erstellen</t>
-  </si>
-  <si>
-    <t>IUserRepository und UserRepositoryDB erweitern (ChangePassword)</t>
-  </si>
-  <si>
-    <t>ChangePassword Methode im UserController erstellen</t>
-  </si>
-  <si>
-    <t>ChangePassword View erstellen</t>
-  </si>
-  <si>
-    <t>IUserRepository und UserRepositoryDB erweitern (ChangeUserData und GetUser)</t>
   </si>
 </sst>
 </file>
@@ -558,7 +561,7 @@
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -614,7 +617,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -643,7 +646,7 @@
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>27</v>
@@ -656,10 +659,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +837,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
@@ -845,7 +848,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
@@ -878,7 +881,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
@@ -892,40 +895,69 @@
         <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>19</v>
+      </c>
+      <c r="D26" s="3">
+        <v>43530</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="3">
+        <v>43531</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="3">
+        <v>43531</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="3">
+        <v>43531</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>44</v>
+      <c r="C30" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IUserRepository und UserRepositoryDB erweitert (ChangePassword)
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
   <si>
     <t>User Stories</t>
   </si>
@@ -662,7 +662,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,12 +947,18 @@
         <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>19</v>
+      </c>
+      <c r="D30" s="3">
+        <v>43531</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UserController erweitert und ChangePassword.cshtml erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>User Stories</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>Navigations-Menü für Zugriff auf das Profil erweitern</t>
-  </si>
-  <si>
-    <t>b</t>
   </si>
 </sst>
 </file>
@@ -662,7 +659,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,12 +955,21 @@
         <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>19</v>
+      </c>
+      <c r="D31" s="3">
+        <v>43531</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="3">
+        <v>43531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UserStory 5 Tasks erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>User Stories</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Navigations-Menü für Zugriff auf das Profil erweitern</t>
+  </si>
+  <si>
+    <t>Grundlegende Karte einbauen</t>
+  </si>
+  <si>
+    <t>Layout anpassen</t>
   </si>
 </sst>
 </file>
@@ -571,7 +577,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,10 +662,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,6 +978,24 @@
         <v>43531</v>
       </c>
     </row>
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Layout für Map angepasst
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t>User Stories</t>
   </si>
@@ -662,7 +662,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,6 +993,12 @@
       <c r="B36" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="3">
+        <v>43545</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UserStory 6 Tasks erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>User Stories</t>
   </si>
@@ -160,6 +160,27 @@
   </si>
   <si>
     <t>Layout anpassen</t>
+  </si>
+  <si>
+    <t>Klasse Booking erstellen</t>
+  </si>
+  <si>
+    <t>Interface IBookingReposittory erstellen</t>
+  </si>
+  <si>
+    <t>Klasse BookingRepository DB erstellen</t>
+  </si>
+  <si>
+    <t>Booking Methode im BookingController erstellen</t>
+  </si>
+  <si>
+    <t>Booking View erstellen</t>
+  </si>
+  <si>
+    <t>email Bestätigung einbauen</t>
+  </si>
+  <si>
+    <t>Tabelle bookings und rooms erstellen</t>
   </si>
 </sst>
 </file>
@@ -574,7 +595,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,10 +680,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,6 +1021,49 @@
         <v>43545</v>
       </c>
     </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tabelle rooms und bookings erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>User Stories</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Tabelle bookings und rooms erstellen</t>
+  </si>
+  <si>
+    <t>bis 28.03.2019</t>
   </si>
 </sst>
 </file>
@@ -682,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,6 +1036,9 @@
       <c r="B39" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
@@ -1052,6 +1058,9 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Booking.cs und IBookingRepository.cs erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>User Stories</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Klasse Booking erstellen</t>
   </si>
   <si>
-    <t>Interface IBookingReposittory erstellen</t>
-  </si>
-  <si>
     <t>Klasse BookingRepository DB erstellen</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>bis 28.03.2019</t>
+  </si>
+  <si>
+    <t>Interface IBookingRepository erstellen</t>
   </si>
 </sst>
 </file>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,43 +1034,58 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" t="s">
         <v>19</v>
+      </c>
+      <c r="D39" s="3">
+        <v>43550</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="3">
+        <v>43550</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="3">
+        <v>43550</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Booking.cshtml und Booking im BookingController erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>User Stories</t>
   </si>
@@ -177,13 +177,16 @@
     <t>Tabelle bookings und rooms erstellen</t>
   </si>
   <si>
-    <t>bis 28.03.2019</t>
-  </si>
-  <si>
     <t>Interface IBookingRepository erstellen</t>
   </si>
   <si>
     <t>Klasse BookingRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>BookingConfirmation Methode im BookingController erstellen</t>
+  </si>
+  <si>
+    <t>BookingConfirmation View erstellen</t>
   </si>
 </sst>
 </file>
@@ -683,10 +686,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1059,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
         <v>19</v>
@@ -1067,7 +1070,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
         <v>19</v>
@@ -1080,17 +1083,36 @@
       <c r="B43" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>53</v>
+      <c r="C43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="3">
+        <v>43557</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="C44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="3">
+        <v>43557</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BookingConfirmation.cshtml und BookingController erweitert
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
   <si>
     <t>User Stories</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Als Benutzer möchte ich den Standort des Hotels sehen und direkt zu Google Maps kommen</t>
   </si>
   <si>
-    <t>Als registrierter Benutzer möchte ich beim Buchen eine email als Bestätigung bekommen</t>
-  </si>
-  <si>
-    <t>Als Benutzer möchte ich alle Seite auf deutsch und englisch aufrufen können</t>
-  </si>
-  <si>
     <t>Priorisierung</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t>Registration Methode im UserController erstellen</t>
   </si>
   <si>
-    <t>Als Admin möchte ich einen eigenen Bereich, wo alle registrierten Benutzer angezeigt und verwaltet werden können</t>
-  </si>
-  <si>
     <t>Als Benutzer möchte ich alle Seiten auf deutsch und englisch aufrufen können</t>
   </si>
   <si>
@@ -171,9 +162,6 @@
     <t>Booking View erstellen</t>
   </si>
   <si>
-    <t>email Bestätigung einbauen</t>
-  </si>
-  <si>
     <t>Tabelle bookings und rooms erstellen</t>
   </si>
   <si>
@@ -187,6 +175,21 @@
   </si>
   <si>
     <t>BookingConfirmation View erstellen</t>
+  </si>
+  <si>
+    <t>User Story in 2 Sprints aufgeteilt</t>
+  </si>
+  <si>
+    <t>Als registrierter Benutzer möchte ich ein Zimmer buchen können wenn ich angemeldet bin</t>
+  </si>
+  <si>
+    <t>Als registrierter Benutzer möchte ich beim buchen die Preise einsehen und eine email als Bestätigung bekommen</t>
+  </si>
+  <si>
+    <t>9.</t>
+  </si>
+  <si>
+    <t>Als Admin möchte ich einen eigenen Bereich, wo alle registrierten Benutzer und Buchungen angezeigt und verwaltet werden können</t>
   </si>
 </sst>
 </file>
@@ -534,16 +537,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -568,12 +571,12 @@
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -583,12 +586,17 @@
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -598,26 +606,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -625,7 +633,7 @@
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -633,7 +641,7 @@
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -641,15 +649,15 @@
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -657,26 +665,34 @@
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -686,35 +702,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="B34" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="61.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -722,10 +739,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>43515</v>
@@ -733,10 +750,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>43515</v>
@@ -744,10 +761,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>43517</v>
@@ -755,7 +772,7 @@
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -763,10 +780,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3">
         <v>43522</v>
@@ -774,10 +791,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="3">
         <v>43522</v>
@@ -785,10 +802,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="3">
         <v>43522</v>
@@ -796,10 +813,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" s="3">
         <v>43522</v>
@@ -807,10 +824,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3">
         <v>43522</v>
@@ -818,10 +835,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14" s="3">
         <v>43522</v>
@@ -829,10 +846,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" s="3">
         <v>43525</v>
@@ -840,7 +857,7 @@
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -848,10 +865,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" s="3">
         <v>43525</v>
@@ -859,10 +876,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" s="3">
         <v>43530</v>
@@ -870,10 +887,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="3">
         <v>43530</v>
@@ -881,10 +898,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21" s="3">
         <v>43530</v>
@@ -892,10 +909,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D22" s="3">
         <v>43530</v>
@@ -903,10 +920,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D23" s="3">
         <v>43530</v>
@@ -914,18 +931,18 @@
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D26" s="3">
         <v>43530</v>
@@ -933,10 +950,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D27" s="3">
         <v>43531</v>
@@ -944,10 +961,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D28" s="3">
         <v>43531</v>
@@ -955,10 +972,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D29" s="3">
         <v>43531</v>
@@ -966,10 +983,10 @@
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D30" s="3">
         <v>43531</v>
@@ -977,10 +994,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D31" s="3">
         <v>43531</v>
@@ -988,132 +1005,150 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D32" s="3">
         <v>43531</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D35" s="3">
         <v>43538</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D36" s="3">
         <v>43545</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D39" s="3">
         <v>43550</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D40" s="3">
         <v>43550</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D41" s="3">
         <v>43550</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D42" s="3">
         <v>43552</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D43" s="3">
         <v>43557</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D44" s="3">
         <v>43557</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="3">
+        <v>43559</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="3">
+        <v>43559</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Insert im BookingRepositoryDB erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="59">
   <si>
     <t>User Stories</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Als Admin möchte ich einen eigenen Bereich, wo alle registrierten Benutzer und Buchungen angezeigt und verwaltet werden können</t>
+  </si>
+  <si>
+    <t>Insert im BookingRepositoryDB erstellen</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,10 +705,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B34" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,11 +1146,22 @@
         <v>43559</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="3">
+        <v>43560</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UserStory 7 tasks erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="63">
   <si>
     <t>User Stories</t>
   </si>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>Insert im BookingRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>GetPrice in IBookingRepository und BookingRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>Price in Booking View einbauen</t>
+  </si>
+  <si>
+    <t>Email Bestätigung bei BookingConfirmation einbauen</t>
+  </si>
+  <si>
+    <t>Price in BookingController einbauen</t>
   </si>
 </sst>
 </file>
@@ -612,7 +624,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,10 +717,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,6 +1177,26 @@
         <v>55</v>
       </c>
     </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Price in BookingController und Booking Views eingebaut
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
   <si>
     <t>User Stories</t>
   </si>
@@ -720,7 +720,7 @@
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,10 +1192,22 @@
       <c r="B51" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="3">
+        <v>43567</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>60</v>
+      </c>
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="3">
+        <v>43567</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UserStory 8 Tasks erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="70">
   <si>
     <t>User Stories</t>
   </si>
@@ -201,10 +201,31 @@
     <t>Price in Booking View einbauen</t>
   </si>
   <si>
-    <t>Email Bestätigung bei BookingConfirmation einbauen</t>
-  </si>
-  <si>
     <t>Price in BookingController einbauen</t>
+  </si>
+  <si>
+    <t>(Email Bestätigung bei BookingConfirmation einbauen)</t>
+  </si>
+  <si>
+    <t>10.</t>
+  </si>
+  <si>
+    <t>Als registrierter Benutzer möchte ich alle Buchungen auf einer eigenen Seite anzeigen lassen</t>
+  </si>
+  <si>
+    <t>GetBookings in BookingRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>ShowBookings View erstellen</t>
+  </si>
+  <si>
+    <t>ShowBookings Methode im BookingController erstellen</t>
+  </si>
+  <si>
+    <t>Als registrierter Benutzer möchte ich alle meine Buchungen auf einer eigenen Seite sehen und löschen können</t>
+  </si>
+  <si>
+    <t>Delete im BookingRepositoryDB erstellen</t>
   </si>
 </sst>
 </file>
@@ -552,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,6 +635,11 @@
         <v>55</v>
       </c>
     </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -621,7 +647,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
@@ -699,7 +725,7 @@
         <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -707,6 +733,14 @@
         <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -717,10 +751,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,7 +1224,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
@@ -1212,7 +1246,35 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GetBookings im BookingRepositoryDB erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="70">
   <si>
     <t>User Stories</t>
   </si>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,6 +1261,12 @@
       <c r="B56" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="3">
+        <v>43567</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">

</xml_diff>

<commit_message>
ShowBookings View und Methode im BookingController erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="70">
   <si>
     <t>User Stories</t>
   </si>
@@ -754,7 +754,7 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,10 +1272,22 @@
       <c r="B57" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="C57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="3">
+        <v>43567</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>66</v>
+      </c>
+      <c r="C58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="3">
+        <v>43567</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Delete im BookingRepositoryDB erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="71">
   <si>
     <t>User Stories</t>
   </si>
@@ -225,7 +225,10 @@
     <t>Als registrierter Benutzer möchte ich alle meine Buchungen auf einer eigenen Seite sehen und löschen können</t>
   </si>
   <si>
-    <t>Delete im BookingRepositoryDB erstellen</t>
+    <t>Delete in IBookingRepository und BookingRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>Delete Methode im BookingsController erstellen</t>
   </si>
 </sst>
 </file>
@@ -751,10 +754,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,6 +1297,17 @@
       <c r="B59" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="3">
+        <v>43572</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Delete Methode im BookingController erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="71">
   <si>
     <t>User Stories</t>
   </si>
@@ -757,7 +757,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,6 +1308,12 @@
       <c r="B60" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="C60" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="3">
+        <v>43573</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UserStory 9 Tasks erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="80">
   <si>
     <t>User Stories</t>
   </si>
@@ -213,9 +213,6 @@
     <t>Als registrierter Benutzer möchte ich alle Buchungen auf einer eigenen Seite anzeigen lassen</t>
   </si>
   <si>
-    <t>GetBookings in BookingRepositoryDB erstellen</t>
-  </si>
-  <si>
     <t>ShowBookings View erstellen</t>
   </si>
   <si>
@@ -225,10 +222,40 @@
     <t>Als registrierter Benutzer möchte ich alle meine Buchungen auf einer eigenen Seite sehen und löschen können</t>
   </si>
   <si>
-    <t>Delete in IBookingRepository und BookingRepositoryDB erstellen</t>
-  </si>
-  <si>
     <t>Delete Methode im BookingsController erstellen</t>
+  </si>
+  <si>
+    <t>GetAllUsers im UserRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>GetBookings im BookingRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>ShowUsers Methode im AdminController erstellen</t>
+  </si>
+  <si>
+    <t>ShowUsers View erstellen</t>
+  </si>
+  <si>
+    <t>Delete im BookingRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>Delete im UserRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>DeleteUser Methode im AdminController erstellen</t>
+  </si>
+  <si>
+    <t>GetAllBookings im BookinRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>ShowBookings Methode im AdminController erstellen</t>
+  </si>
+  <si>
+    <t>DeleteBooking Methode im AdminController erstellen</t>
+  </si>
+  <si>
+    <t>(Delete bereits im BookingRepositoryDB vorhanden)</t>
   </si>
 </sst>
 </file>
@@ -653,7 +680,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,10 +781,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,12 +1284,12 @@
         <v>34</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C56" t="s">
         <v>17</v>
@@ -1273,7 +1300,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" t="s">
         <v>17</v>
@@ -1284,7 +1311,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
         <v>17</v>
@@ -1295,7 +1322,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C59" t="s">
         <v>17</v>
@@ -1306,13 +1333,71 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C60" t="s">
         <v>17</v>
       </c>
       <c r="D60" s="3">
         <v>43573</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GetAllUsers im UserRepositoryDB erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
   <si>
     <t>User Stories</t>
   </si>
@@ -783,7 +783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
       <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
@@ -1354,6 +1354,12 @@
       <c r="B63" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="C63" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="3">
+        <v>43573</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">

</xml_diff>

<commit_message>
ShowUsers View und Methode im AdminController erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="80">
   <si>
     <t>User Stories</t>
   </si>
@@ -784,7 +784,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,43 +1365,55 @@
       <c r="B64" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="3">
+        <v>43574</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="3">
+        <v>43574</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Delete im UserRepositoryDB erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="80">
   <si>
     <t>User Stories</t>
   </si>
@@ -784,7 +784,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,6 +1387,12 @@
       <c r="B66" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="C66" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="3">
+        <v>43574</v>
+      </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">

</xml_diff>

<commit_message>
GetAllBookings im BookingRepositoryDB erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="80">
   <si>
     <t>User Stories</t>
   </si>
@@ -246,9 +246,6 @@
     <t>DeleteUser Methode im AdminController erstellen</t>
   </si>
   <si>
-    <t>GetAllBookings im BookinRepositoryDB erstellen</t>
-  </si>
-  <si>
     <t>ShowBookings Methode im AdminController erstellen</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>(Delete bereits im BookingRepositoryDB vorhanden)</t>
+  </si>
+  <si>
+    <t>GetAllBookings im BookingRepositoryDB erstellen</t>
   </si>
 </sst>
 </file>
@@ -784,7 +784,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,15 +1398,27 @@
       <c r="B67" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="C67" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="3">
+        <v>43574</v>
+      </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="C68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68" s="3">
+        <v>43574</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
@@ -1416,12 +1428,12 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ShowBookings View und Methode im AdminController erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="80">
   <si>
     <t>User Stories</t>
   </si>
@@ -784,7 +784,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,6 +1420,12 @@
       <c r="B69" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="C69" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="3">
+        <v>43579</v>
+      </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">

</xml_diff>

<commit_message>
DeleteBooking im AdminController erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="80">
   <si>
     <t>User Stories</t>
   </si>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,6 +1431,12 @@
       <c r="B70" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C70" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="3">
+        <v>43579</v>
+      </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">

</xml_diff>

<commit_message>
SetPrices im BookingRepositoryDB erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="82">
   <si>
     <t>User Stories</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Als registrierter Benutzer möchte ich ein Zimmer buchen können wenn ich angemeldet bin</t>
   </si>
   <si>
-    <t>Als registrierter Benutzer möchte ich beim buchen die Preise einsehen und eine email als Bestätigung bekommen</t>
-  </si>
-  <si>
     <t>9.</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
     <t>Price in BookingController einbauen</t>
   </si>
   <si>
-    <t>(Email Bestätigung bei BookingConfirmation einbauen)</t>
-  </si>
-  <si>
     <t>10.</t>
   </si>
   <si>
@@ -256,6 +250,18 @@
   </si>
   <si>
     <t>GetAllBookings im BookingRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>Als registrierter Benutzer möchte ich beim buchen die Preise für alle Zimmer und den Preis meiner Buchung einsehen</t>
+  </si>
+  <si>
+    <t>SetPrice Methode im AdminController erstellen</t>
+  </si>
+  <si>
+    <t>SetPriceView erstellen</t>
+  </si>
+  <si>
+    <t>SetPrices im BookingRepositoryDB erstellen</t>
   </si>
 </sst>
 </file>
@@ -606,7 +612,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +648,7 @@
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -662,12 +668,12 @@
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -680,7 +686,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +753,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -755,20 +761,20 @@
         <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
@@ -781,10 +787,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1230,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s">
         <v>17</v>
@@ -1238,12 +1244,12 @@
         <v>12</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" t="s">
         <v>17</v>
@@ -1254,7 +1260,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
@@ -1265,7 +1271,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C52" t="s">
         <v>17</v>
@@ -1274,22 +1280,28 @@
         <v>43567</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>34</v>
       </c>
+      <c r="B54" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="3">
+        <v>43567</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
         <v>17</v>
@@ -1300,7 +1312,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C57" t="s">
         <v>17</v>
@@ -1311,43 +1323,43 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
         <v>17</v>
       </c>
       <c r="D58" s="3">
-        <v>43567</v>
+        <v>43572</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C59" t="s">
         <v>17</v>
       </c>
       <c r="D59" s="3">
-        <v>43572</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C60" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" s="3">
         <v>43573</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>55</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>56</v>
       </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
+      </c>
+      <c r="C62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="3">
+        <v>43573</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1358,12 +1370,12 @@
         <v>17</v>
       </c>
       <c r="D63" s="3">
-        <v>43573</v>
+        <v>43574</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
         <v>17</v>
@@ -1385,7 +1397,7 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C66" t="s">
         <v>17</v>
@@ -1396,7 +1408,7 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C67" t="s">
         <v>17</v>
@@ -1407,18 +1419,18 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C68" t="s">
         <v>17</v>
       </c>
       <c r="D68" s="3">
-        <v>43574</v>
+        <v>43579</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C69" t="s">
         <v>17</v>
@@ -1429,23 +1441,42 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C70" t="s">
         <v>17</v>
-      </c>
-      <c r="D70" s="3">
-        <v>43579</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C71" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="3">
+        <v>43579</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
+      </c>
+      <c r="C72" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72" s="3">
+        <v>43579</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SetPrices View und Methode im AdminController erstellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="79">
   <si>
     <t>User Stories</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Registration Methode im UserController erstellen</t>
   </si>
   <si>
-    <t>Als Benutzer möchte ich alle Seiten auf deutsch und englisch aufrufen können</t>
-  </si>
-  <si>
     <t>für Erfolgsseiten Klasse und View Message erstellen</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>BookingConfirmation View erstellen</t>
   </si>
   <si>
-    <t>User Story in 2 Sprints aufgeteilt</t>
-  </si>
-  <si>
     <t>Als registrierter Benutzer möchte ich ein Zimmer buchen können wenn ich angemeldet bin</t>
   </si>
   <si>
@@ -201,9 +195,6 @@
     <t>Price in BookingController einbauen</t>
   </si>
   <si>
-    <t>10.</t>
-  </si>
-  <si>
     <t>Als registrierter Benutzer möchte ich alle Buchungen auf einer eigenen Seite anzeigen lassen</t>
   </si>
   <si>
@@ -255,13 +246,13 @@
     <t>Als registrierter Benutzer möchte ich beim buchen die Preise für alle Zimmer und den Preis meiner Buchung einsehen</t>
   </si>
   <si>
-    <t>SetPrice Methode im AdminController erstellen</t>
-  </si>
-  <si>
-    <t>SetPriceView erstellen</t>
-  </si>
-  <si>
     <t>SetPrices im BookingRepositoryDB erstellen</t>
+  </si>
+  <si>
+    <t>SetPrices Methode im AdminController erstellen</t>
+  </si>
+  <si>
+    <t>SetPrices View erstellen</t>
   </si>
 </sst>
 </file>
@@ -609,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,12 +634,12 @@
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -658,22 +649,17 @@
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -683,10 +669,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +715,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -745,7 +731,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -753,31 +739,23 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -789,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,10 +786,10 @@
         <v>13</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -931,7 +909,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -950,7 +928,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -961,7 +939,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -972,7 +950,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -983,7 +961,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -994,7 +972,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1005,7 +983,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1019,12 +997,12 @@
         <v>9</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
@@ -1035,7 +1013,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
@@ -1046,7 +1024,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
@@ -1057,7 +1035,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -1068,7 +1046,7 @@
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -1079,7 +1057,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
@@ -1090,7 +1068,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
@@ -1109,7 +1087,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
@@ -1120,7 +1098,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
@@ -1134,15 +1112,13 @@
         <v>11</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
@@ -1153,7 +1129,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
         <v>17</v>
@@ -1164,7 +1140,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" t="s">
         <v>17</v>
@@ -1175,7 +1151,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C42" t="s">
         <v>17</v>
@@ -1186,7 +1162,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
@@ -1197,7 +1173,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
         <v>17</v>
@@ -1208,7 +1184,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
         <v>17</v>
@@ -1219,7 +1195,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" t="s">
         <v>17</v>
@@ -1230,7 +1206,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C47" t="s">
         <v>17</v>
@@ -1239,17 +1215,17 @@
         <v>43560</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>12</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C50" t="s">
         <v>17</v>
@@ -1258,9 +1234,9 @@
         <v>43567</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
@@ -1269,9 +1245,9 @@
         <v>43567</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
         <v>17</v>
@@ -1280,17 +1256,17 @@
         <v>43567</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C55" t="s">
         <v>17</v>
@@ -1299,9 +1275,9 @@
         <v>43567</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C56" t="s">
         <v>17</v>
@@ -1310,9 +1286,9 @@
         <v>43567</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C57" t="s">
         <v>17</v>
@@ -1321,9 +1297,9 @@
         <v>43567</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s">
         <v>17</v>
@@ -1332,9 +1308,9 @@
         <v>43572</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C59" t="s">
         <v>17</v>
@@ -1343,17 +1319,18 @@
         <v>43573</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C62" t="s">
         <v>17</v>
@@ -1362,9 +1339,9 @@
         <v>43573</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C63" t="s">
         <v>17</v>
@@ -1373,9 +1350,9 @@
         <v>43574</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C64" t="s">
         <v>17</v>
@@ -1386,7 +1363,7 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
         <v>17</v>
@@ -1397,7 +1374,7 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C66" t="s">
         <v>17</v>
@@ -1408,7 +1385,7 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C67" t="s">
         <v>17</v>
@@ -1419,7 +1396,7 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
         <v>17</v>
@@ -1430,7 +1407,7 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C69" t="s">
         <v>17</v>
@@ -1441,7 +1418,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C70" t="s">
         <v>17</v>
@@ -1449,7 +1426,7 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C71" t="s">
         <v>17</v>
@@ -1460,7 +1437,7 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C72" t="s">
         <v>17</v>
@@ -1471,12 +1448,24 @@
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="C73" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="3">
+        <v>43579</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="C74" t="s">
+        <v>17</v>
+      </c>
+      <c r="D74" s="3">
+        <v>43579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>